<commit_message>
process department related details added
</commit_message>
<xml_diff>
--- a/documents/templates/bulk-upload/01-BulkUploadDepartment.xlsx
+++ b/documents/templates/bulk-upload/01-BulkUploadDepartment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineshgajjar/Documents/Work/GitLab/YHWorks/Briot/clients/TMML/server/documents/templates/bulk-upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B578A67-A57F-294E-937E-13D32BDE3716}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CEF71B-636F-564B-87DC-539E399F7F2A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="16040" xr2:uid="{56435790-24FB-C04B-A0DB-B752F92072DE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>departnment Name</t>
   </si>
@@ -39,9 +39,6 @@
     <t>IT</t>
   </si>
   <si>
-    <t>Planning and Production</t>
-  </si>
-  <si>
     <t>SCM</t>
   </si>
   <si>
@@ -49,6 +46,12 @@
   </si>
   <si>
     <t>Factory Maintenance</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>Production Planning and Control</t>
   </si>
 </sst>
 </file>
@@ -403,15 +406,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44911B77-7284-6F4B-A3A7-9629A9AD25BA}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -427,22 +430,27 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
production department employees added
</commit_message>
<xml_diff>
--- a/documents/templates/bulk-upload/01-BulkUploadDepartment.xlsx
+++ b/documents/templates/bulk-upload/01-BulkUploadDepartment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineshgajjar/Documents/Work/GitLab/YHWorks/Briot/clients/TMML/server/documents/templates/bulk-upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CEF71B-636F-564B-87DC-539E399F7F2A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C896C9F-0FCA-F448-B17C-1E4A387B09EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="16040" xr2:uid="{56435790-24FB-C04B-A0DB-B752F92072DE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>departnment Name</t>
   </si>
@@ -52,14 +52,25 @@
   </si>
   <si>
     <t>Production Planning and Control</t>
+  </si>
+  <si>
+    <t>Machine Shop (Production)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -87,9 +98,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -406,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44911B77-7284-6F4B-A3A7-9629A9AD25BA}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -429,7 +441,7 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -444,13 +456,18 @@
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>